<commit_message>
Added first part of first objective
</commit_message>
<xml_diff>
--- a/Schedule Objective 1/patientdata_objective_1.xlsx
+++ b/Schedule Objective 1/patientdata_objective_1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="2058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="2401">
   <si>
     <t>Room_No</t>
   </si>
@@ -4084,6 +4084,1035 @@
   </si>
   <si>
     <t>Evans</t>
+  </si>
+  <si>
+    <t>Özçivit</t>
+  </si>
+  <si>
+    <t>Portman</t>
+  </si>
+  <si>
+    <t>Timberlake</t>
+  </si>
+  <si>
+    <t>Seinfeld</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Evcen</t>
+  </si>
+  <si>
+    <t>Brando</t>
+  </si>
+  <si>
+    <t>Boz</t>
+  </si>
+  <si>
+    <t>Costanza</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Dalkılıç</t>
+  </si>
+  <si>
+    <t>Hiddleston</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Patient_Priority</t>
+  </si>
+  <si>
+    <t>Operation_Day</t>
+  </si>
+  <si>
+    <t>Room_No</t>
+  </si>
+  <si>
+    <t>Available_Interval</t>
+  </si>
+  <si>
+    <t>(60,220)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(40,160)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(140,220)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(180,360)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(0,200)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(100,380)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(180,260)</t>
+  </si>
+  <si>
+    <t>(140,300)</t>
+  </si>
+  <si>
+    <t>(80,160)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(40,220)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(320,360)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(240,480)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(300,480)</t>
+  </si>
+  <si>
+    <t>(280,420)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(60,120)</t>
+  </si>
+  <si>
+    <t>(40,140)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(140,300)</t>
+  </si>
+  <si>
+    <t>(100,180)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(20,80)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(80,220)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(140,360)</t>
+  </si>
+  <si>
+    <t>(60,140)</t>
+  </si>
+  <si>
+    <t>(280,340)</t>
+  </si>
+  <si>
+    <t>(360,460)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(80,260)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(160,440)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(180,340)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(160,200)</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Sched_Interval</t>
+  </si>
+  <si>
+    <t>(60,160)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(20,100)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(240,300)</t>
+  </si>
+  <si>
+    <t>(440,480)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(360,440)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(140,180)</t>
+  </si>
+  <si>
+    <t>(280,320)</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(180,300)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(300,340)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(380,480)</t>
+  </si>
+  <si>
+    <t>(380,440)</t>
+  </si>
+  <si>
+    <t>(300,320)</t>
+  </si>
+  <si>
+    <t>(260,380)</t>
+  </si>
+  <si>
+    <t>(220,280)</t>
+  </si>
+  <si>
+    <t>(180,220)</t>
+  </si>
+  <si>
+    <t>(280,320)</t>
+  </si>
+  <si>
+    <t>(200,240)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(120,160)</t>
+  </si>
+  <si>
+    <t>(320,440)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(140,160)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(340,440)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(300,360)</t>
+  </si>
+  <si>
+    <t>(260,280)</t>
+  </si>
+  <si>
+    <t>(220,240)</t>
+  </si>
+  <si>
+    <t>(100,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(180,300)</t>
+  </si>
+  <si>
+    <t>(120,160)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(60,80)</t>
+  </si>
+  <si>
+    <t>(220,260)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(460,480)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(340,440)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(100,140)</t>
+  </si>
+  <si>
+    <t>(320,340)</t>
+  </si>
+  <si>
+    <t>(360,420)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(380,460)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(340,400)</t>
+  </si>
+  <si>
+    <t>(260,300)</t>
+  </si>
+  <si>
+    <t>(260,380)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(300,360)</t>
+  </si>
+  <si>
+    <t>(400,460)</t>
+  </si>
+  <si>
+    <t>(220,340)</t>
+  </si>
+  <si>
+    <t>(200,260)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>Patient_Name</t>
+  </si>
+  <si>
+    <t>Milo</t>
+  </si>
+  <si>
+    <t>Kenan</t>
+  </si>
+  <si>
+    <t>Cosmo</t>
+  </si>
+  <si>
+    <t>Aras Bulut</t>
+  </si>
+  <si>
+    <t>Serenay</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Yıldız</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Cillian</t>
+  </si>
+  <si>
+    <t>Sherlock</t>
+  </si>
+  <si>
+    <t>Ata</t>
+  </si>
+  <si>
+    <t>Hannibal</t>
+  </si>
+  <si>
+    <t>Haluk</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Rosamund</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Ezgi</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Hugh</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Ali Rıza</t>
+  </si>
+  <si>
+    <t>Özge</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Ramsay</t>
+  </si>
+  <si>
+    <t>Sezen</t>
+  </si>
+  <si>
+    <t>Gülse</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Ragnar</t>
+  </si>
+  <si>
+    <t>Aleyna</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Sylvester</t>
+  </si>
+  <si>
+    <t>Kıvanç</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Tarkan</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Tyrion</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Dwayne</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Hayko</t>
+  </si>
+  <si>
+    <t>Elçin</t>
+  </si>
+  <si>
+    <t>Nihal</t>
+  </si>
+  <si>
+    <t>Merve</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Hande</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Bellatrix</t>
+  </si>
+  <si>
+    <t>Hülya</t>
+  </si>
+  <si>
+    <t>Ivana</t>
+  </si>
+  <si>
+    <t>Keira</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Çağatay</t>
+  </si>
+  <si>
+    <t>Demet</t>
+  </si>
+  <si>
+    <t>Tom Marvolo</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Bihter</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>Burak</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Fahriye</t>
+  </si>
+  <si>
+    <t>Marlon</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>Patient_Surname</t>
+  </si>
+  <si>
+    <t>Ventimiglia</t>
+  </si>
+  <si>
+    <t>Doğulu</t>
+  </si>
+  <si>
+    <t>Kramer</t>
+  </si>
+  <si>
+    <t>İynemli</t>
+  </si>
+  <si>
+    <t>Sarıkaya</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Tilbe</t>
+  </si>
+  <si>
+    <t>Damon</t>
+  </si>
+  <si>
+    <t>Murphy</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>Demirer</t>
+  </si>
+  <si>
+    <t>Lecter</t>
+  </si>
+  <si>
+    <t>Levent</t>
+  </si>
+  <si>
+    <t>Hathaway</t>
+  </si>
+  <si>
+    <t>Pike</t>
+  </si>
+  <si>
+    <t>Radcliffe</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Pitt</t>
+  </si>
+  <si>
+    <t>Mola</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Hardy</t>
+  </si>
+  <si>
+    <t>Jackman</t>
+  </si>
+  <si>
+    <t>Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Tekin</t>
+  </si>
+  <si>
+    <t>Özpirinççi</t>
+  </si>
+  <si>
+    <t>Weaving</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>Aksu</t>
+  </si>
+  <si>
+    <t>Birsel</t>
+  </si>
+  <si>
+    <t>Cavill</t>
+  </si>
+  <si>
+    <t>Lothbrok</t>
+  </si>
+  <si>
+    <t>Tilki</t>
+  </si>
+  <si>
+    <t>Robbie</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>Stallone</t>
+  </si>
+  <si>
+    <t>Tatlıtuğ</t>
+  </si>
+  <si>
+    <t>Downey Jr.</t>
+  </si>
+  <si>
+    <t>DiCaprio</t>
+  </si>
+  <si>
+    <t>Tevetoğlu</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Jolie</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>O'Dowd</t>
+  </si>
+  <si>
+    <t>Lannister</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t>Fiennes</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Moriarty</t>
+  </si>
+  <si>
+    <t>Cepkin</t>
+  </si>
+  <si>
+    <t>Sangu</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Boluğur</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Erçel</t>
+  </si>
+  <si>
+    <t>Winslet</t>
+  </si>
+  <si>
+    <t>Lestrange</t>
+  </si>
+  <si>
+    <t>Avşar</t>
+  </si>
+  <si>
+    <t>Sert</t>
+  </si>
+  <si>
+    <t>Knightley</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Ulusoy</t>
+  </si>
+  <si>
+    <t>Akalın</t>
+  </si>
+  <si>
+    <t>Riddle</t>
+  </si>
+  <si>
+    <t>Clooney</t>
+  </si>
+  <si>
+    <t>Baggins</t>
+  </si>
+  <si>
+    <t>Chappelle</t>
+  </si>
+  <si>
+    <t>Carrey</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Schrute</t>
   </si>
   <si>
     <t>Özçivit</t>
@@ -6247,28 +7276,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1715</v>
+        <v>2058</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1716</v>
+        <v>2059</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1801</v>
+        <v>2144</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1802</v>
+        <v>2145</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1884</v>
+        <v>2227</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1970</v>
+        <v>2313</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>2056</v>
+        <v>2399</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>2057</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="2">
@@ -6276,19 +7305,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1717</v>
+        <v>2060</v>
       </c>
       <c r="C2" s="0">
         <v>100</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1803</v>
+        <v>2146</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1885</v>
+        <v>2228</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1971</v>
+        <v>2314</v>
       </c>
       <c r="G2" s="0">
         <v>1</v>
@@ -6302,19 +7331,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1718</v>
+        <v>2061</v>
       </c>
       <c r="C3" s="0">
         <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1804</v>
+        <v>2147</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1886</v>
+        <v>2229</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1972</v>
+        <v>2315</v>
       </c>
       <c r="G3" s="0">
         <v>1</v>
@@ -6328,19 +7357,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1719</v>
+        <v>2062</v>
       </c>
       <c r="C4" s="0">
         <v>80</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1805</v>
+        <v>2148</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1887</v>
+        <v>2230</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1973</v>
+        <v>2316</v>
       </c>
       <c r="G4" s="0">
         <v>1</v>
@@ -6354,19 +7383,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1720</v>
+        <v>2063</v>
       </c>
       <c r="C5" s="0">
         <v>60</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1806</v>
+        <v>2149</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1888</v>
+        <v>2231</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1974</v>
+        <v>2317</v>
       </c>
       <c r="G5" s="0">
         <v>1</v>
@@ -6380,19 +7409,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1721</v>
+        <v>2064</v>
       </c>
       <c r="C6" s="0">
         <v>60</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1807</v>
+        <v>2150</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1889</v>
+        <v>2232</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1975</v>
+        <v>2318</v>
       </c>
       <c r="G6" s="0">
         <v>1</v>
@@ -6406,19 +7435,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1722</v>
+        <v>2065</v>
       </c>
       <c r="C7" s="0">
         <v>40</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1808</v>
+        <v>2151</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1890</v>
+        <v>2233</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1976</v>
+        <v>2319</v>
       </c>
       <c r="G7" s="0">
         <v>1</v>
@@ -6432,19 +7461,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1723</v>
+        <v>2066</v>
       </c>
       <c r="C8" s="0">
         <v>80</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1809</v>
+        <v>2152</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1891</v>
+        <v>2234</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1977</v>
+        <v>2320</v>
       </c>
       <c r="G8" s="0">
         <v>2</v>
@@ -6458,19 +7487,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1724</v>
+        <v>2067</v>
       </c>
       <c r="C9" s="0">
         <v>80</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1809</v>
+        <v>2152</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1892</v>
+        <v>2235</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1978</v>
+        <v>2321</v>
       </c>
       <c r="G9" s="0">
         <v>2</v>
@@ -6484,19 +7513,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1725</v>
+        <v>2068</v>
       </c>
       <c r="C10" s="0">
         <v>80</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1810</v>
+        <v>2153</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1893</v>
+        <v>2236</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1979</v>
+        <v>2322</v>
       </c>
       <c r="G10" s="0">
         <v>2</v>
@@ -6510,19 +7539,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1726</v>
+        <v>2069</v>
       </c>
       <c r="C11" s="0">
         <v>80</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1811</v>
+        <v>2154</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1894</v>
+        <v>2237</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1980</v>
+        <v>2323</v>
       </c>
       <c r="G11" s="0">
         <v>2</v>
@@ -6536,19 +7565,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1727</v>
+        <v>2070</v>
       </c>
       <c r="C12" s="0">
         <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1812</v>
+        <v>2155</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1895</v>
+        <v>2238</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1981</v>
+        <v>2324</v>
       </c>
       <c r="G12" s="0">
         <v>2</v>
@@ -6562,19 +7591,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1728</v>
+        <v>2071</v>
       </c>
       <c r="C13" s="0">
         <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1813</v>
+        <v>2156</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1896</v>
+        <v>2239</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1982</v>
+        <v>2325</v>
       </c>
       <c r="G13" s="0">
         <v>2</v>
@@ -6588,19 +7617,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1729</v>
+        <v>2072</v>
       </c>
       <c r="C14" s="0">
         <v>40</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1814</v>
+        <v>2157</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1897</v>
+        <v>2240</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1983</v>
+        <v>2326</v>
       </c>
       <c r="G14" s="0">
         <v>2</v>
@@ -6614,19 +7643,19 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1730</v>
+        <v>2073</v>
       </c>
       <c r="C15" s="0">
         <v>40</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1815</v>
+        <v>2158</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1898</v>
+        <v>2241</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1984</v>
+        <v>2327</v>
       </c>
       <c r="G15" s="0">
         <v>2</v>
@@ -6640,19 +7669,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1731</v>
+        <v>2074</v>
       </c>
       <c r="C16" s="0">
         <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1816</v>
+        <v>2159</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>1899</v>
+        <v>2242</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1985</v>
+        <v>2328</v>
       </c>
       <c r="G16" s="0">
         <v>2</v>
@@ -6666,19 +7695,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1732</v>
+        <v>2075</v>
       </c>
       <c r="C17" s="0">
         <v>120</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1817</v>
+        <v>2160</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>1900</v>
+        <v>2243</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1986</v>
+        <v>2329</v>
       </c>
       <c r="G17" s="0">
         <v>3</v>
@@ -6692,19 +7721,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1733</v>
+        <v>2076</v>
       </c>
       <c r="C18" s="0">
         <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1818</v>
+        <v>2161</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>1901</v>
+        <v>2244</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1987</v>
+        <v>2330</v>
       </c>
       <c r="G18" s="0">
         <v>3</v>
@@ -6718,19 +7747,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1734</v>
+        <v>2077</v>
       </c>
       <c r="C19" s="0">
         <v>40</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1819</v>
+        <v>2162</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1902</v>
+        <v>2245</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1988</v>
+        <v>2331</v>
       </c>
       <c r="G19" s="0">
         <v>4</v>
@@ -6744,19 +7773,19 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>1735</v>
+        <v>2078</v>
       </c>
       <c r="C20" s="0">
         <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1820</v>
+        <v>2163</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>1903</v>
+        <v>2246</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1989</v>
+        <v>2332</v>
       </c>
       <c r="G20" s="0">
         <v>4</v>
@@ -6770,19 +7799,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1736</v>
+        <v>2079</v>
       </c>
       <c r="C21" s="0">
         <v>80</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1821</v>
+        <v>2164</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>1904</v>
+        <v>2247</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1990</v>
+        <v>2333</v>
       </c>
       <c r="G21" s="0">
         <v>0</v>
@@ -6796,19 +7825,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1737</v>
+        <v>2080</v>
       </c>
       <c r="C22" s="0">
         <v>120</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1822</v>
+        <v>2165</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>1905</v>
+        <v>2248</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1991</v>
+        <v>2334</v>
       </c>
       <c r="G22" s="0">
         <v>1</v>
@@ -6822,19 +7851,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1738</v>
+        <v>2081</v>
       </c>
       <c r="C23" s="0">
         <v>120</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>1822</v>
+        <v>2165</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1906</v>
+        <v>2249</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1992</v>
+        <v>2335</v>
       </c>
       <c r="G23" s="0">
         <v>1</v>
@@ -6848,19 +7877,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1739</v>
+        <v>2082</v>
       </c>
       <c r="C24" s="0">
         <v>100</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>1823</v>
+        <v>2166</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>1907</v>
+        <v>2250</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1993</v>
+        <v>2336</v>
       </c>
       <c r="G24" s="0">
         <v>1</v>
@@ -6874,19 +7903,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1740</v>
+        <v>2083</v>
       </c>
       <c r="C25" s="0">
         <v>100</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>1824</v>
+        <v>2167</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>1908</v>
+        <v>2251</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1994</v>
+        <v>2337</v>
       </c>
       <c r="G25" s="0">
         <v>1</v>
@@ -6900,19 +7929,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1741</v>
+        <v>2084</v>
       </c>
       <c r="C26" s="0">
         <v>60</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1825</v>
+        <v>2168</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1909</v>
+        <v>2252</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1995</v>
+        <v>2338</v>
       </c>
       <c r="G26" s="0">
         <v>1</v>
@@ -6926,19 +7955,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1742</v>
+        <v>2085</v>
       </c>
       <c r="C27" s="0">
         <v>20</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1826</v>
+        <v>2169</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1910</v>
+        <v>2253</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1996</v>
+        <v>2339</v>
       </c>
       <c r="G27" s="0">
         <v>1</v>
@@ -6952,19 +7981,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1743</v>
+        <v>2086</v>
       </c>
       <c r="C28" s="0">
         <v>120</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>1827</v>
+        <v>2170</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1911</v>
+        <v>2254</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1997</v>
+        <v>2340</v>
       </c>
       <c r="G28" s="0">
         <v>2</v>
@@ -6978,19 +8007,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1744</v>
+        <v>2087</v>
       </c>
       <c r="C29" s="0">
         <v>60</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1828</v>
+        <v>2171</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>1912</v>
+        <v>2255</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1998</v>
+        <v>2341</v>
       </c>
       <c r="G29" s="0">
         <v>2</v>
@@ -7004,19 +8033,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>1745</v>
+        <v>2088</v>
       </c>
       <c r="C30" s="0">
         <v>40</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1829</v>
+        <v>2172</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>1913</v>
+        <v>2256</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>1999</v>
+        <v>2342</v>
       </c>
       <c r="G30" s="0">
         <v>2</v>
@@ -7030,19 +8059,19 @@
         <v>3</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>1746</v>
+        <v>2089</v>
       </c>
       <c r="C31" s="0">
         <v>40</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1830</v>
+        <v>2173</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>1914</v>
+        <v>2257</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>2000</v>
+        <v>2343</v>
       </c>
       <c r="G31" s="0">
         <v>2</v>
@@ -7056,19 +8085,19 @@
         <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>1747</v>
+        <v>2090</v>
       </c>
       <c r="C32" s="0">
         <v>40</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1831</v>
+        <v>2174</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>1915</v>
+        <v>2258</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>2001</v>
+        <v>2344</v>
       </c>
       <c r="G32" s="0">
         <v>2</v>
@@ -7082,19 +8111,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1748</v>
+        <v>2091</v>
       </c>
       <c r="C33" s="0">
         <v>120</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1832</v>
+        <v>2175</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>1916</v>
+        <v>2259</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>2002</v>
+        <v>2345</v>
       </c>
       <c r="G33" s="0">
         <v>3</v>
@@ -7108,19 +8137,19 @@
         <v>2</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>1749</v>
+        <v>2092</v>
       </c>
       <c r="C34" s="0">
         <v>40</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1833</v>
+        <v>2176</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>1917</v>
+        <v>2260</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>2003</v>
+        <v>2346</v>
       </c>
       <c r="G34" s="0">
         <v>3</v>
@@ -7134,19 +8163,19 @@
         <v>3</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>1750</v>
+        <v>2093</v>
       </c>
       <c r="C35" s="0">
         <v>120</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>1834</v>
+        <v>2177</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>1918</v>
+        <v>2261</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>2004</v>
+        <v>2347</v>
       </c>
       <c r="G35" s="0">
         <v>4</v>
@@ -7160,19 +8189,19 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>1751</v>
+        <v>2094</v>
       </c>
       <c r="C36" s="0">
         <v>20</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>1835</v>
+        <v>2178</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>1919</v>
+        <v>2262</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>2005</v>
+        <v>2348</v>
       </c>
       <c r="G36" s="0">
         <v>4</v>
@@ -7186,19 +8215,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>1752</v>
+        <v>2095</v>
       </c>
       <c r="C37" s="0">
         <v>120</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>1836</v>
+        <v>2179</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>1920</v>
+        <v>2263</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>2006</v>
+        <v>2349</v>
       </c>
       <c r="G37" s="0">
         <v>0</v>
@@ -7212,19 +8241,19 @@
         <v>2</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>1753</v>
+        <v>2096</v>
       </c>
       <c r="C38" s="0">
         <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>1837</v>
+        <v>2180</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>1921</v>
+        <v>2264</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>2007</v>
+        <v>2350</v>
       </c>
       <c r="G38" s="0">
         <v>0</v>
@@ -7238,19 +8267,19 @@
         <v>3</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>1754</v>
+        <v>2097</v>
       </c>
       <c r="C39" s="0">
         <v>80</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1838</v>
+        <v>2181</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>1922</v>
+        <v>2265</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>2008</v>
+        <v>2351</v>
       </c>
       <c r="G39" s="0">
         <v>0</v>
@@ -7264,19 +8293,19 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>1755</v>
+        <v>2098</v>
       </c>
       <c r="C40" s="0">
         <v>100</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>1839</v>
+        <v>2182</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>1923</v>
+        <v>2266</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>2009</v>
+        <v>2352</v>
       </c>
       <c r="G40" s="0">
         <v>1</v>
@@ -7290,19 +8319,19 @@
         <v>2</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>1756</v>
+        <v>2099</v>
       </c>
       <c r="C41" s="0">
         <v>100</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>1840</v>
+        <v>2183</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>1924</v>
+        <v>2267</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>2010</v>
+        <v>2353</v>
       </c>
       <c r="G41" s="0">
         <v>1</v>
@@ -7316,19 +8345,19 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>1757</v>
+        <v>2100</v>
       </c>
       <c r="C42" s="0">
         <v>100</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>1841</v>
+        <v>2184</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>1925</v>
+        <v>2268</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>2011</v>
+        <v>2354</v>
       </c>
       <c r="G42" s="0">
         <v>1</v>
@@ -7342,19 +8371,19 @@
         <v>3</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>1758</v>
+        <v>2101</v>
       </c>
       <c r="C43" s="0">
         <v>20</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>1842</v>
+        <v>2185</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>1926</v>
+        <v>2269</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>2012</v>
+        <v>2355</v>
       </c>
       <c r="G43" s="0">
         <v>1</v>
@@ -7368,19 +8397,19 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>1759</v>
+        <v>2102</v>
       </c>
       <c r="C44" s="0">
         <v>20</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1843</v>
+        <v>2186</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>1927</v>
+        <v>2270</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>2013</v>
+        <v>2356</v>
       </c>
       <c r="G44" s="0">
         <v>1</v>
@@ -7394,19 +8423,19 @@
         <v>3</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>1760</v>
+        <v>2103</v>
       </c>
       <c r="C45" s="0">
         <v>20</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1844</v>
+        <v>2187</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>1928</v>
+        <v>2271</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>2014</v>
+        <v>2357</v>
       </c>
       <c r="G45" s="0">
         <v>1</v>
@@ -7420,19 +8449,19 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>1761</v>
+        <v>2104</v>
       </c>
       <c r="C46" s="0">
         <v>120</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1845</v>
+        <v>2188</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>1929</v>
+        <v>2272</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>2015</v>
+        <v>2358</v>
       </c>
       <c r="G46" s="0">
         <v>2</v>
@@ -7446,19 +8475,19 @@
         <v>2</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>1762</v>
+        <v>2105</v>
       </c>
       <c r="C47" s="0">
         <v>100</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1846</v>
+        <v>2189</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>1930</v>
+        <v>2273</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>2016</v>
+        <v>2359</v>
       </c>
       <c r="G47" s="0">
         <v>2</v>
@@ -7472,19 +8501,19 @@
         <v>3</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>1763</v>
+        <v>2106</v>
       </c>
       <c r="C48" s="0">
         <v>120</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1847</v>
+        <v>2190</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>1931</v>
+        <v>2274</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>2017</v>
+        <v>2360</v>
       </c>
       <c r="G48" s="0">
         <v>3</v>
@@ -7498,19 +8527,19 @@
         <v>3</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>1764</v>
+        <v>2107</v>
       </c>
       <c r="C49" s="0">
         <v>60</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1848</v>
+        <v>2191</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>1932</v>
+        <v>2275</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>2018</v>
+        <v>2361</v>
       </c>
       <c r="G49" s="0">
         <v>3</v>
@@ -7524,19 +8553,19 @@
         <v>2</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>1765</v>
+        <v>2108</v>
       </c>
       <c r="C50" s="0">
         <v>20</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1849</v>
+        <v>2192</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>1933</v>
+        <v>2276</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>2019</v>
+        <v>2362</v>
       </c>
       <c r="G50" s="0">
         <v>3</v>
@@ -7550,19 +8579,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>1766</v>
+        <v>2109</v>
       </c>
       <c r="C51" s="0">
         <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1850</v>
+        <v>2193</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>1934</v>
+        <v>2277</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>2020</v>
+        <v>2363</v>
       </c>
       <c r="G51" s="0">
         <v>4</v>
@@ -7576,19 +8605,19 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>1767</v>
+        <v>2110</v>
       </c>
       <c r="C52" s="0">
         <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>1851</v>
+        <v>2194</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>1935</v>
+        <v>2278</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>2021</v>
+        <v>2364</v>
       </c>
       <c r="G52" s="0">
         <v>4</v>
@@ -7602,19 +8631,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>1768</v>
+        <v>2111</v>
       </c>
       <c r="C53" s="0">
         <v>20</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>1851</v>
+        <v>2194</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>1936</v>
+        <v>2279</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>2022</v>
+        <v>2365</v>
       </c>
       <c r="G53" s="0">
         <v>4</v>
@@ -7628,19 +8657,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>1769</v>
+        <v>2112</v>
       </c>
       <c r="C54" s="0">
         <v>100</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1852</v>
+        <v>2195</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>1937</v>
+        <v>2280</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>2023</v>
+        <v>2366</v>
       </c>
       <c r="G54" s="0">
         <v>0</v>
@@ -7654,19 +8683,19 @@
         <v>2</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>1769</v>
+        <v>2112</v>
       </c>
       <c r="C55" s="0">
         <v>100</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>1852</v>
+        <v>2195</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>1938</v>
+        <v>2281</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>2024</v>
+        <v>2367</v>
       </c>
       <c r="G55" s="0">
         <v>0</v>
@@ -7680,19 +8709,19 @@
         <v>3</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1770</v>
+        <v>2113</v>
       </c>
       <c r="C56" s="0">
         <v>60</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>1853</v>
+        <v>2196</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>1939</v>
+        <v>2282</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>2025</v>
+        <v>2368</v>
       </c>
       <c r="G56" s="0">
         <v>0</v>
@@ -7706,19 +8735,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>1771</v>
+        <v>2114</v>
       </c>
       <c r="C57" s="0">
         <v>120</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>1854</v>
+        <v>2197</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>1940</v>
+        <v>2283</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>2026</v>
+        <v>2369</v>
       </c>
       <c r="G57" s="0">
         <v>1</v>
@@ -7732,19 +8761,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>1772</v>
+        <v>2115</v>
       </c>
       <c r="C58" s="0">
         <v>40</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>1855</v>
+        <v>2198</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>1941</v>
+        <v>2284</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>2027</v>
+        <v>2370</v>
       </c>
       <c r="G58" s="0">
         <v>1</v>
@@ -7758,19 +8787,19 @@
         <v>3</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>1773</v>
+        <v>2116</v>
       </c>
       <c r="C59" s="0">
         <v>20</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>1856</v>
+        <v>2199</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>1942</v>
+        <v>2285</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>2028</v>
+        <v>2371</v>
       </c>
       <c r="G59" s="0">
         <v>1</v>
@@ -7784,19 +8813,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>1774</v>
+        <v>2117</v>
       </c>
       <c r="C60" s="0">
         <v>20</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>1857</v>
+        <v>2200</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>1943</v>
+        <v>2286</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>2029</v>
+        <v>2372</v>
       </c>
       <c r="G60" s="0">
         <v>1</v>
@@ -7810,19 +8839,19 @@
         <v>3</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>1775</v>
+        <v>2118</v>
       </c>
       <c r="C61" s="0">
         <v>20</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>1858</v>
+        <v>2201</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>1944</v>
+        <v>2287</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>2030</v>
+        <v>2373</v>
       </c>
       <c r="G61" s="0">
         <v>1</v>
@@ -7836,19 +8865,19 @@
         <v>2</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>1776</v>
+        <v>2119</v>
       </c>
       <c r="C62" s="0">
         <v>40</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>1859</v>
+        <v>2202</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>1945</v>
+        <v>2288</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>2031</v>
+        <v>2374</v>
       </c>
       <c r="G62" s="0">
         <v>2</v>
@@ -7862,19 +8891,19 @@
         <v>1</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>1777</v>
+        <v>2120</v>
       </c>
       <c r="C63" s="0">
         <v>20</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>1860</v>
+        <v>2203</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>1946</v>
+        <v>2289</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>2032</v>
+        <v>2375</v>
       </c>
       <c r="G63" s="0">
         <v>2</v>
@@ -7888,19 +8917,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>1778</v>
+        <v>2121</v>
       </c>
       <c r="C64" s="0">
         <v>20</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>1861</v>
+        <v>2204</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>1947</v>
+        <v>2290</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>2033</v>
+        <v>2376</v>
       </c>
       <c r="G64" s="0">
         <v>2</v>
@@ -7914,19 +8943,19 @@
         <v>2</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>1779</v>
+        <v>2122</v>
       </c>
       <c r="C65" s="0">
         <v>100</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>1862</v>
+        <v>2205</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>1948</v>
+        <v>2291</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>2034</v>
+        <v>2377</v>
       </c>
       <c r="G65" s="0">
         <v>3</v>
@@ -7940,19 +8969,19 @@
         <v>2</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>1780</v>
+        <v>2123</v>
       </c>
       <c r="C66" s="0">
         <v>100</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>1863</v>
+        <v>2206</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>1949</v>
+        <v>2292</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>2035</v>
+        <v>2378</v>
       </c>
       <c r="G66" s="0">
         <v>3</v>
@@ -7966,19 +8995,19 @@
         <v>3</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>1781</v>
+        <v>2124</v>
       </c>
       <c r="C67" s="0">
         <v>100</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>1864</v>
+        <v>2207</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>1950</v>
+        <v>2293</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>2036</v>
+        <v>2379</v>
       </c>
       <c r="G67" s="0">
         <v>3</v>
@@ -7992,19 +9021,19 @@
         <v>3</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>1782</v>
+        <v>2125</v>
       </c>
       <c r="C68" s="0">
         <v>40</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>1865</v>
+        <v>2208</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>1951</v>
+        <v>2294</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>2037</v>
+        <v>2380</v>
       </c>
       <c r="G68" s="0">
         <v>3</v>
@@ -8018,19 +9047,19 @@
         <v>1</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>1783</v>
+        <v>2126</v>
       </c>
       <c r="C69" s="0">
         <v>20</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>1866</v>
+        <v>2209</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>1952</v>
+        <v>2295</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>2038</v>
+        <v>2381</v>
       </c>
       <c r="G69" s="0">
         <v>3</v>
@@ -8044,19 +9073,19 @@
         <v>1</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>1784</v>
+        <v>2127</v>
       </c>
       <c r="C70" s="0">
         <v>60</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>1867</v>
+        <v>2210</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>1953</v>
+        <v>2296</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>2039</v>
+        <v>2382</v>
       </c>
       <c r="G70" s="0">
         <v>4</v>
@@ -8070,19 +9099,19 @@
         <v>1</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>1785</v>
+        <v>2128</v>
       </c>
       <c r="C71" s="0">
         <v>120</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>1868</v>
+        <v>2211</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>1954</v>
+        <v>2297</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>2040</v>
+        <v>2383</v>
       </c>
       <c r="G71" s="0">
         <v>0</v>
@@ -8096,19 +9125,19 @@
         <v>2</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>1786</v>
+        <v>2129</v>
       </c>
       <c r="C72" s="0">
         <v>100</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>1869</v>
+        <v>2212</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>1955</v>
+        <v>2298</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>2041</v>
+        <v>2384</v>
       </c>
       <c r="G72" s="0">
         <v>0</v>
@@ -8122,19 +9151,19 @@
         <v>3</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>1787</v>
+        <v>2130</v>
       </c>
       <c r="C73" s="0">
         <v>60</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>1870</v>
+        <v>2213</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>1956</v>
+        <v>2299</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>2042</v>
+        <v>2385</v>
       </c>
       <c r="G73" s="0">
         <v>0</v>
@@ -8148,19 +9177,19 @@
         <v>1</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>1788</v>
+        <v>2131</v>
       </c>
       <c r="C74" s="0">
         <v>120</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>1871</v>
+        <v>2214</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>1957</v>
+        <v>2300</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>2043</v>
+        <v>2386</v>
       </c>
       <c r="G74" s="0">
         <v>1</v>
@@ -8174,19 +9203,19 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>1789</v>
+        <v>2132</v>
       </c>
       <c r="C75" s="0">
         <v>100</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>1872</v>
+        <v>2215</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>1958</v>
+        <v>2301</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>2044</v>
+        <v>2387</v>
       </c>
       <c r="G75" s="0">
         <v>1</v>
@@ -8200,19 +9229,19 @@
         <v>2</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>1790</v>
+        <v>2133</v>
       </c>
       <c r="C76" s="0">
         <v>80</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>1873</v>
+        <v>2216</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>1959</v>
+        <v>2302</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>2045</v>
+        <v>2388</v>
       </c>
       <c r="G76" s="0">
         <v>1</v>
@@ -8226,19 +9255,19 @@
         <v>2</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>1791</v>
+        <v>2134</v>
       </c>
       <c r="C77" s="0">
         <v>60</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>1874</v>
+        <v>2217</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>1960</v>
+        <v>2303</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>2046</v>
+        <v>2389</v>
       </c>
       <c r="G77" s="0">
         <v>1</v>
@@ -8252,19 +9281,19 @@
         <v>3</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>1792</v>
+        <v>2135</v>
       </c>
       <c r="C78" s="0">
         <v>60</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>1875</v>
+        <v>2218</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>1961</v>
+        <v>2304</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>2047</v>
+        <v>2390</v>
       </c>
       <c r="G78" s="0">
         <v>1</v>
@@ -8278,19 +9307,19 @@
         <v>1</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>1793</v>
+        <v>2136</v>
       </c>
       <c r="C79" s="0">
         <v>40</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>1876</v>
+        <v>2219</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>1962</v>
+        <v>2305</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>2048</v>
+        <v>2391</v>
       </c>
       <c r="G79" s="0">
         <v>1</v>
@@ -8304,19 +9333,19 @@
         <v>2</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>1794</v>
+        <v>2137</v>
       </c>
       <c r="C80" s="0">
         <v>120</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>1877</v>
+        <v>2220</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>1963</v>
+        <v>2306</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>2049</v>
+        <v>2392</v>
       </c>
       <c r="G80" s="0">
         <v>2</v>
@@ -8330,19 +9359,19 @@
         <v>1</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>1795</v>
+        <v>2138</v>
       </c>
       <c r="C81" s="0">
         <v>100</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>1878</v>
+        <v>2221</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>1964</v>
+        <v>2307</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>2050</v>
+        <v>2393</v>
       </c>
       <c r="G81" s="0">
         <v>2</v>
@@ -8356,19 +9385,19 @@
         <v>1</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>1796</v>
+        <v>2139</v>
       </c>
       <c r="C82" s="0">
         <v>60</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>1879</v>
+        <v>2222</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>1965</v>
+        <v>2308</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>2051</v>
+        <v>2394</v>
       </c>
       <c r="G82" s="0">
         <v>2</v>
@@ -8382,19 +9411,19 @@
         <v>3</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>1797</v>
+        <v>2140</v>
       </c>
       <c r="C83" s="0">
         <v>60</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>1880</v>
+        <v>2223</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>1966</v>
+        <v>2309</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>2052</v>
+        <v>2395</v>
       </c>
       <c r="G83" s="0">
         <v>2</v>
@@ -8408,19 +9437,19 @@
         <v>3</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>1798</v>
+        <v>2141</v>
       </c>
       <c r="C84" s="0">
         <v>120</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>1881</v>
+        <v>2224</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>1967</v>
+        <v>2310</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>2053</v>
+        <v>2396</v>
       </c>
       <c r="G84" s="0">
         <v>3</v>
@@ -8434,19 +9463,19 @@
         <v>2</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>1799</v>
+        <v>2142</v>
       </c>
       <c r="C85" s="0">
         <v>60</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>1882</v>
+        <v>2225</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>1968</v>
+        <v>2311</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>2054</v>
+        <v>2397</v>
       </c>
       <c r="G85" s="0">
         <v>3</v>
@@ -8460,19 +9489,19 @@
         <v>2</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>1800</v>
+        <v>2143</v>
       </c>
       <c r="C86" s="0">
         <v>20</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>1883</v>
+        <v>2226</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>1969</v>
+        <v>2312</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>2055</v>
+        <v>2398</v>
       </c>
       <c r="G86" s="0">
         <v>4</v>

</xml_diff>

<commit_message>
Added appendix to the report
</commit_message>
<xml_diff>
--- a/Schedule Objective 1/patientdata_objective_1.xlsx
+++ b/Schedule Objective 1/patientdata_objective_1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6960" uniqueCount="6860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7308" uniqueCount="7203">
   <si>
     <t>Room_No</t>
   </si>
@@ -4084,6 +4084,1035 @@
   </si>
   <si>
     <t>Evans</t>
+  </si>
+  <si>
+    <t>Özçivit</t>
+  </si>
+  <si>
+    <t>Portman</t>
+  </si>
+  <si>
+    <t>Timberlake</t>
+  </si>
+  <si>
+    <t>Seinfeld</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Evcen</t>
+  </si>
+  <si>
+    <t>Brando</t>
+  </si>
+  <si>
+    <t>Boz</t>
+  </si>
+  <si>
+    <t>Costanza</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Dalkılıç</t>
+  </si>
+  <si>
+    <t>Hiddleston</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Patient_Priority</t>
+  </si>
+  <si>
+    <t>Operation_Day</t>
+  </si>
+  <si>
+    <t>Room_No</t>
+  </si>
+  <si>
+    <t>Available_Interval</t>
+  </si>
+  <si>
+    <t>(60,220)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(40,160)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(140,220)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(180,360)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(0,200)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(100,380)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(180,260)</t>
+  </si>
+  <si>
+    <t>(140,300)</t>
+  </si>
+  <si>
+    <t>(80,160)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(40,220)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(320,360)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(240,480)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(300,480)</t>
+  </si>
+  <si>
+    <t>(280,420)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(60,120)</t>
+  </si>
+  <si>
+    <t>(40,140)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(140,300)</t>
+  </si>
+  <si>
+    <t>(100,180)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(20,80)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(80,220)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(140,360)</t>
+  </si>
+  <si>
+    <t>(60,140)</t>
+  </si>
+  <si>
+    <t>(280,340)</t>
+  </si>
+  <si>
+    <t>(360,460)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(80,260)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(160,440)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(180,340)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(160,200)</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Sched_Interval</t>
+  </si>
+  <si>
+    <t>(60,160)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(20,100)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(240,300)</t>
+  </si>
+  <si>
+    <t>(440,480)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(360,440)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(140,180)</t>
+  </si>
+  <si>
+    <t>(280,320)</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(180,300)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(300,340)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(380,480)</t>
+  </si>
+  <si>
+    <t>(380,440)</t>
+  </si>
+  <si>
+    <t>(300,320)</t>
+  </si>
+  <si>
+    <t>(260,380)</t>
+  </si>
+  <si>
+    <t>(220,280)</t>
+  </si>
+  <si>
+    <t>(180,220)</t>
+  </si>
+  <si>
+    <t>(280,320)</t>
+  </si>
+  <si>
+    <t>(200,240)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(120,160)</t>
+  </si>
+  <si>
+    <t>(320,440)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(140,160)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(340,440)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(300,360)</t>
+  </si>
+  <si>
+    <t>(260,280)</t>
+  </si>
+  <si>
+    <t>(220,240)</t>
+  </si>
+  <si>
+    <t>(100,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(180,300)</t>
+  </si>
+  <si>
+    <t>(120,160)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(60,80)</t>
+  </si>
+  <si>
+    <t>(220,260)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(460,480)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(340,440)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(100,140)</t>
+  </si>
+  <si>
+    <t>(320,340)</t>
+  </si>
+  <si>
+    <t>(360,420)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(380,460)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(340,400)</t>
+  </si>
+  <si>
+    <t>(260,300)</t>
+  </si>
+  <si>
+    <t>(260,380)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(300,360)</t>
+  </si>
+  <si>
+    <t>(400,460)</t>
+  </si>
+  <si>
+    <t>(220,340)</t>
+  </si>
+  <si>
+    <t>(200,260)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>Patient_Name</t>
+  </si>
+  <si>
+    <t>Milo</t>
+  </si>
+  <si>
+    <t>Kenan</t>
+  </si>
+  <si>
+    <t>Cosmo</t>
+  </si>
+  <si>
+    <t>Aras Bulut</t>
+  </si>
+  <si>
+    <t>Serenay</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Yıldız</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Cillian</t>
+  </si>
+  <si>
+    <t>Sherlock</t>
+  </si>
+  <si>
+    <t>Ata</t>
+  </si>
+  <si>
+    <t>Hannibal</t>
+  </si>
+  <si>
+    <t>Haluk</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Rosamund</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Ezgi</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Hugh</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Ali Rıza</t>
+  </si>
+  <si>
+    <t>Özge</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Ramsay</t>
+  </si>
+  <si>
+    <t>Sezen</t>
+  </si>
+  <si>
+    <t>Gülse</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Ragnar</t>
+  </si>
+  <si>
+    <t>Aleyna</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Sylvester</t>
+  </si>
+  <si>
+    <t>Kıvanç</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Tarkan</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Tyrion</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Dwayne</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Hayko</t>
+  </si>
+  <si>
+    <t>Elçin</t>
+  </si>
+  <si>
+    <t>Nihal</t>
+  </si>
+  <si>
+    <t>Merve</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Hande</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Bellatrix</t>
+  </si>
+  <si>
+    <t>Hülya</t>
+  </si>
+  <si>
+    <t>Ivana</t>
+  </si>
+  <si>
+    <t>Keira</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Çağatay</t>
+  </si>
+  <si>
+    <t>Demet</t>
+  </si>
+  <si>
+    <t>Tom Marvolo</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Bihter</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>Burak</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Fahriye</t>
+  </si>
+  <si>
+    <t>Marlon</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>Patient_Surname</t>
+  </si>
+  <si>
+    <t>Ventimiglia</t>
+  </si>
+  <si>
+    <t>Doğulu</t>
+  </si>
+  <si>
+    <t>Kramer</t>
+  </si>
+  <si>
+    <t>İynemli</t>
+  </si>
+  <si>
+    <t>Sarıkaya</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Tilbe</t>
+  </si>
+  <si>
+    <t>Damon</t>
+  </si>
+  <si>
+    <t>Murphy</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>Demirer</t>
+  </si>
+  <si>
+    <t>Lecter</t>
+  </si>
+  <si>
+    <t>Levent</t>
+  </si>
+  <si>
+    <t>Hathaway</t>
+  </si>
+  <si>
+    <t>Pike</t>
+  </si>
+  <si>
+    <t>Radcliffe</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Pitt</t>
+  </si>
+  <si>
+    <t>Mola</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Hardy</t>
+  </si>
+  <si>
+    <t>Jackman</t>
+  </si>
+  <si>
+    <t>Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Tekin</t>
+  </si>
+  <si>
+    <t>Özpirinççi</t>
+  </si>
+  <si>
+    <t>Weaving</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>Aksu</t>
+  </si>
+  <si>
+    <t>Birsel</t>
+  </si>
+  <si>
+    <t>Cavill</t>
+  </si>
+  <si>
+    <t>Lothbrok</t>
+  </si>
+  <si>
+    <t>Tilki</t>
+  </si>
+  <si>
+    <t>Robbie</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>Stallone</t>
+  </si>
+  <si>
+    <t>Tatlıtuğ</t>
+  </si>
+  <si>
+    <t>Downey Jr.</t>
+  </si>
+  <si>
+    <t>DiCaprio</t>
+  </si>
+  <si>
+    <t>Tevetoğlu</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Jolie</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>O'Dowd</t>
+  </si>
+  <si>
+    <t>Lannister</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t>Fiennes</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Moriarty</t>
+  </si>
+  <si>
+    <t>Cepkin</t>
+  </si>
+  <si>
+    <t>Sangu</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Boluğur</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Erçel</t>
+  </si>
+  <si>
+    <t>Winslet</t>
+  </si>
+  <si>
+    <t>Lestrange</t>
+  </si>
+  <si>
+    <t>Avşar</t>
+  </si>
+  <si>
+    <t>Sert</t>
+  </si>
+  <si>
+    <t>Knightley</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Ulusoy</t>
+  </si>
+  <si>
+    <t>Akalın</t>
+  </si>
+  <si>
+    <t>Riddle</t>
+  </si>
+  <si>
+    <t>Clooney</t>
+  </si>
+  <si>
+    <t>Baggins</t>
+  </si>
+  <si>
+    <t>Chappelle</t>
+  </si>
+  <si>
+    <t>Carrey</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Schrute</t>
   </si>
   <si>
     <t>Özçivit</t>
@@ -20641,40 +21670,40 @@
   <dimension ref="A1:H86"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="true"/>
-    <col min="2" max="2" width="17.28515625" customWidth="true"/>
-    <col min="3" max="3" width="8.85546875" customWidth="true"/>
-    <col min="4" max="4" width="14.28515625" customWidth="true"/>
-    <col min="5" max="5" width="13.85546875" customWidth="true"/>
-    <col min="6" max="6" width="16.42578125" customWidth="true"/>
-    <col min="7" max="7" width="15.140625" customWidth="true"/>
-    <col min="8" max="8" width="14.42578125" customWidth="true"/>
+    <col min="1" max="1" width="9.44140625" customWidth="true"/>
+    <col min="2" max="2" width="16.07421875" customWidth="true"/>
+    <col min="3" max="3" width="8.53125" customWidth="true"/>
+    <col min="4" max="4" width="13.44140625" customWidth="true"/>
+    <col min="5" max="5" width="12.89453125" customWidth="true"/>
+    <col min="6" max="6" width="15.44140625" customWidth="true"/>
+    <col min="7" max="7" width="13.984375" customWidth="true"/>
+    <col min="8" max="8" width="13.8046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>6517</v>
+        <v>6860</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6518</v>
+        <v>6861</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>6603</v>
+        <v>6946</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>6604</v>
+        <v>6947</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6686</v>
+        <v>7029</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>6772</v>
+        <v>7115</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6858</v>
+        <v>7201</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6859</v>
+        <v>7202</v>
       </c>
     </row>
     <row r="2">
@@ -20682,19 +21711,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6519</v>
+        <v>6862</v>
       </c>
       <c r="C2" s="0">
         <v>100</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6605</v>
+        <v>6948</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6687</v>
+        <v>7030</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6773</v>
+        <v>7116</v>
       </c>
       <c r="G2" s="0">
         <v>1</v>
@@ -20708,19 +21737,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6520</v>
+        <v>6863</v>
       </c>
       <c r="C3" s="0">
         <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6606</v>
+        <v>6949</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6688</v>
+        <v>7031</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>6774</v>
+        <v>7117</v>
       </c>
       <c r="G3" s="0">
         <v>1</v>
@@ -20734,19 +21763,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6521</v>
+        <v>6864</v>
       </c>
       <c r="C4" s="0">
         <v>80</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6607</v>
+        <v>6950</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>6689</v>
+        <v>7032</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>6775</v>
+        <v>7118</v>
       </c>
       <c r="G4" s="0">
         <v>1</v>
@@ -20760,19 +21789,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6522</v>
+        <v>6865</v>
       </c>
       <c r="C5" s="0">
         <v>60</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>6608</v>
+        <v>6951</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>6690</v>
+        <v>7033</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>6776</v>
+        <v>7119</v>
       </c>
       <c r="G5" s="0">
         <v>1</v>
@@ -20786,19 +21815,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6523</v>
+        <v>6866</v>
       </c>
       <c r="C6" s="0">
         <v>60</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>6609</v>
+        <v>6952</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>6691</v>
+        <v>7034</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>6777</v>
+        <v>7120</v>
       </c>
       <c r="G6" s="0">
         <v>1</v>
@@ -20812,19 +21841,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6524</v>
+        <v>6867</v>
       </c>
       <c r="C7" s="0">
         <v>40</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>6610</v>
+        <v>6953</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>6692</v>
+        <v>7035</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>6778</v>
+        <v>7121</v>
       </c>
       <c r="G7" s="0">
         <v>1</v>
@@ -20838,19 +21867,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>6525</v>
+        <v>6868</v>
       </c>
       <c r="C8" s="0">
         <v>80</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>6611</v>
+        <v>6954</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>6693</v>
+        <v>7036</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>6779</v>
+        <v>7122</v>
       </c>
       <c r="G8" s="0">
         <v>2</v>
@@ -20864,19 +21893,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>6526</v>
+        <v>6869</v>
       </c>
       <c r="C9" s="0">
         <v>80</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>6611</v>
+        <v>6954</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>6694</v>
+        <v>7037</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>6780</v>
+        <v>7123</v>
       </c>
       <c r="G9" s="0">
         <v>2</v>
@@ -20890,19 +21919,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>6527</v>
+        <v>6870</v>
       </c>
       <c r="C10" s="0">
         <v>80</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>6612</v>
+        <v>6955</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>6695</v>
+        <v>7038</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>6781</v>
+        <v>7124</v>
       </c>
       <c r="G10" s="0">
         <v>2</v>
@@ -20916,19 +21945,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>6528</v>
+        <v>6871</v>
       </c>
       <c r="C11" s="0">
         <v>80</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>6613</v>
+        <v>6956</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>6696</v>
+        <v>7039</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>6782</v>
+        <v>7125</v>
       </c>
       <c r="G11" s="0">
         <v>2</v>
@@ -20942,19 +21971,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>6529</v>
+        <v>6872</v>
       </c>
       <c r="C12" s="0">
         <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>6614</v>
+        <v>6957</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>6697</v>
+        <v>7040</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>6783</v>
+        <v>7126</v>
       </c>
       <c r="G12" s="0">
         <v>2</v>
@@ -20968,19 +21997,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>6530</v>
+        <v>6873</v>
       </c>
       <c r="C13" s="0">
         <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>6615</v>
+        <v>6958</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>6698</v>
+        <v>7041</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>6784</v>
+        <v>7127</v>
       </c>
       <c r="G13" s="0">
         <v>2</v>
@@ -20994,19 +22023,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>6531</v>
+        <v>6874</v>
       </c>
       <c r="C14" s="0">
         <v>40</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>6616</v>
+        <v>6959</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>6699</v>
+        <v>7042</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>6785</v>
+        <v>7128</v>
       </c>
       <c r="G14" s="0">
         <v>2</v>
@@ -21020,19 +22049,19 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>6532</v>
+        <v>6875</v>
       </c>
       <c r="C15" s="0">
         <v>40</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>6617</v>
+        <v>6960</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>6700</v>
+        <v>7043</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>6786</v>
+        <v>7129</v>
       </c>
       <c r="G15" s="0">
         <v>2</v>
@@ -21046,19 +22075,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>6533</v>
+        <v>6876</v>
       </c>
       <c r="C16" s="0">
         <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>6618</v>
+        <v>6961</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>6701</v>
+        <v>7044</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>6787</v>
+        <v>7130</v>
       </c>
       <c r="G16" s="0">
         <v>2</v>
@@ -21072,19 +22101,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>6534</v>
+        <v>6877</v>
       </c>
       <c r="C17" s="0">
         <v>120</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>6619</v>
+        <v>6962</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>6702</v>
+        <v>7045</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>6788</v>
+        <v>7131</v>
       </c>
       <c r="G17" s="0">
         <v>3</v>
@@ -21098,19 +22127,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>6535</v>
+        <v>6878</v>
       </c>
       <c r="C18" s="0">
         <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>6620</v>
+        <v>6963</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>6703</v>
+        <v>7046</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>6789</v>
+        <v>7132</v>
       </c>
       <c r="G18" s="0">
         <v>3</v>
@@ -21124,19 +22153,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>6536</v>
+        <v>6879</v>
       </c>
       <c r="C19" s="0">
         <v>40</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>6621</v>
+        <v>6964</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>6704</v>
+        <v>7047</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>6790</v>
+        <v>7133</v>
       </c>
       <c r="G19" s="0">
         <v>4</v>
@@ -21150,19 +22179,19 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>6537</v>
+        <v>6880</v>
       </c>
       <c r="C20" s="0">
         <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>6622</v>
+        <v>6965</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>6705</v>
+        <v>7048</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>6791</v>
+        <v>7134</v>
       </c>
       <c r="G20" s="0">
         <v>4</v>
@@ -21176,19 +22205,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>6538</v>
+        <v>6881</v>
       </c>
       <c r="C21" s="0">
         <v>80</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>6623</v>
+        <v>6966</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>6706</v>
+        <v>7049</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>6792</v>
+        <v>7135</v>
       </c>
       <c r="G21" s="0">
         <v>0</v>
@@ -21202,19 +22231,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>6539</v>
+        <v>6882</v>
       </c>
       <c r="C22" s="0">
         <v>120</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>6624</v>
+        <v>6967</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>6707</v>
+        <v>7050</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>6793</v>
+        <v>7136</v>
       </c>
       <c r="G22" s="0">
         <v>1</v>
@@ -21228,19 +22257,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>6540</v>
+        <v>6883</v>
       </c>
       <c r="C23" s="0">
         <v>120</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>6624</v>
+        <v>6967</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>6708</v>
+        <v>7051</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>6794</v>
+        <v>7137</v>
       </c>
       <c r="G23" s="0">
         <v>1</v>
@@ -21254,19 +22283,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>6541</v>
+        <v>6884</v>
       </c>
       <c r="C24" s="0">
         <v>100</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>6625</v>
+        <v>6968</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>6709</v>
+        <v>7052</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>6795</v>
+        <v>7138</v>
       </c>
       <c r="G24" s="0">
         <v>1</v>
@@ -21280,19 +22309,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>6542</v>
+        <v>6885</v>
       </c>
       <c r="C25" s="0">
         <v>100</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>6626</v>
+        <v>6969</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>6710</v>
+        <v>7053</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>6796</v>
+        <v>7139</v>
       </c>
       <c r="G25" s="0">
         <v>1</v>
@@ -21306,19 +22335,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>6543</v>
+        <v>6886</v>
       </c>
       <c r="C26" s="0">
         <v>60</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>6627</v>
+        <v>6970</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>6711</v>
+        <v>7054</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>6797</v>
+        <v>7140</v>
       </c>
       <c r="G26" s="0">
         <v>1</v>
@@ -21332,19 +22361,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>6544</v>
+        <v>6887</v>
       </c>
       <c r="C27" s="0">
         <v>20</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>6628</v>
+        <v>6971</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>6712</v>
+        <v>7055</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>6798</v>
+        <v>7141</v>
       </c>
       <c r="G27" s="0">
         <v>1</v>
@@ -21358,19 +22387,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>6545</v>
+        <v>6888</v>
       </c>
       <c r="C28" s="0">
         <v>120</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>6629</v>
+        <v>6972</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>6713</v>
+        <v>7056</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>6799</v>
+        <v>7142</v>
       </c>
       <c r="G28" s="0">
         <v>2</v>
@@ -21384,19 +22413,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>6546</v>
+        <v>6889</v>
       </c>
       <c r="C29" s="0">
         <v>60</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>6630</v>
+        <v>6973</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>6714</v>
+        <v>7057</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>6800</v>
+        <v>7143</v>
       </c>
       <c r="G29" s="0">
         <v>2</v>
@@ -21410,19 +22439,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>6547</v>
+        <v>6890</v>
       </c>
       <c r="C30" s="0">
         <v>40</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>6631</v>
+        <v>6974</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>6715</v>
+        <v>7058</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>6801</v>
+        <v>7144</v>
       </c>
       <c r="G30" s="0">
         <v>2</v>
@@ -21436,19 +22465,19 @@
         <v>3</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>6548</v>
+        <v>6891</v>
       </c>
       <c r="C31" s="0">
         <v>40</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>6632</v>
+        <v>6975</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>6716</v>
+        <v>7059</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>6802</v>
+        <v>7145</v>
       </c>
       <c r="G31" s="0">
         <v>2</v>
@@ -21462,19 +22491,19 @@
         <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>6549</v>
+        <v>6892</v>
       </c>
       <c r="C32" s="0">
         <v>40</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>6633</v>
+        <v>6976</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>6717</v>
+        <v>7060</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>6803</v>
+        <v>7146</v>
       </c>
       <c r="G32" s="0">
         <v>2</v>
@@ -21488,19 +22517,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>6550</v>
+        <v>6893</v>
       </c>
       <c r="C33" s="0">
         <v>120</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>6634</v>
+        <v>6977</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>6718</v>
+        <v>7061</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>6804</v>
+        <v>7147</v>
       </c>
       <c r="G33" s="0">
         <v>3</v>
@@ -21514,19 +22543,19 @@
         <v>2</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>6551</v>
+        <v>6894</v>
       </c>
       <c r="C34" s="0">
         <v>40</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>6635</v>
+        <v>6978</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>6719</v>
+        <v>7062</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>6805</v>
+        <v>7148</v>
       </c>
       <c r="G34" s="0">
         <v>3</v>
@@ -21540,19 +22569,19 @@
         <v>3</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>6552</v>
+        <v>6895</v>
       </c>
       <c r="C35" s="0">
         <v>120</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>6636</v>
+        <v>6979</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>6720</v>
+        <v>7063</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>6806</v>
+        <v>7149</v>
       </c>
       <c r="G35" s="0">
         <v>4</v>
@@ -21566,19 +22595,19 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>6553</v>
+        <v>6896</v>
       </c>
       <c r="C36" s="0">
         <v>20</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>6637</v>
+        <v>6980</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>6721</v>
+        <v>7064</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>6807</v>
+        <v>7150</v>
       </c>
       <c r="G36" s="0">
         <v>4</v>
@@ -21592,19 +22621,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>6554</v>
+        <v>6897</v>
       </c>
       <c r="C37" s="0">
         <v>120</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>6638</v>
+        <v>6981</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>6722</v>
+        <v>7065</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>6808</v>
+        <v>7151</v>
       </c>
       <c r="G37" s="0">
         <v>0</v>
@@ -21618,19 +22647,19 @@
         <v>2</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>6555</v>
+        <v>6898</v>
       </c>
       <c r="C38" s="0">
         <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>6639</v>
+        <v>6982</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>6723</v>
+        <v>7066</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>6809</v>
+        <v>7152</v>
       </c>
       <c r="G38" s="0">
         <v>0</v>
@@ -21644,19 +22673,19 @@
         <v>3</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>6556</v>
+        <v>6899</v>
       </c>
       <c r="C39" s="0">
         <v>80</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>6640</v>
+        <v>6983</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>6724</v>
+        <v>7067</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>6810</v>
+        <v>7153</v>
       </c>
       <c r="G39" s="0">
         <v>0</v>
@@ -21670,19 +22699,19 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>6557</v>
+        <v>6900</v>
       </c>
       <c r="C40" s="0">
         <v>100</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>6641</v>
+        <v>6984</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>6725</v>
+        <v>7068</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>6811</v>
+        <v>7154</v>
       </c>
       <c r="G40" s="0">
         <v>1</v>
@@ -21696,19 +22725,19 @@
         <v>2</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>6558</v>
+        <v>6901</v>
       </c>
       <c r="C41" s="0">
         <v>100</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>6642</v>
+        <v>6985</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>6726</v>
+        <v>7069</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>6812</v>
+        <v>7155</v>
       </c>
       <c r="G41" s="0">
         <v>1</v>
@@ -21722,19 +22751,19 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>6559</v>
+        <v>6902</v>
       </c>
       <c r="C42" s="0">
         <v>100</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>6643</v>
+        <v>6986</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>6727</v>
+        <v>7070</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>6813</v>
+        <v>7156</v>
       </c>
       <c r="G42" s="0">
         <v>1</v>
@@ -21748,19 +22777,19 @@
         <v>3</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>6560</v>
+        <v>6903</v>
       </c>
       <c r="C43" s="0">
         <v>20</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>6644</v>
+        <v>6987</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>6728</v>
+        <v>7071</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>6814</v>
+        <v>7157</v>
       </c>
       <c r="G43" s="0">
         <v>1</v>
@@ -21774,19 +22803,19 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>6561</v>
+        <v>6904</v>
       </c>
       <c r="C44" s="0">
         <v>20</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>6645</v>
+        <v>6988</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>6729</v>
+        <v>7072</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>6815</v>
+        <v>7158</v>
       </c>
       <c r="G44" s="0">
         <v>1</v>
@@ -21800,19 +22829,19 @@
         <v>3</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>6562</v>
+        <v>6905</v>
       </c>
       <c r="C45" s="0">
         <v>20</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>6646</v>
+        <v>6989</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>6730</v>
+        <v>7073</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>6816</v>
+        <v>7159</v>
       </c>
       <c r="G45" s="0">
         <v>1</v>
@@ -21826,19 +22855,19 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>6563</v>
+        <v>6906</v>
       </c>
       <c r="C46" s="0">
         <v>120</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>6647</v>
+        <v>6990</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>6731</v>
+        <v>7074</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>6817</v>
+        <v>7160</v>
       </c>
       <c r="G46" s="0">
         <v>2</v>
@@ -21852,19 +22881,19 @@
         <v>2</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>6564</v>
+        <v>6907</v>
       </c>
       <c r="C47" s="0">
         <v>100</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>6648</v>
+        <v>6991</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>6732</v>
+        <v>7075</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>6818</v>
+        <v>7161</v>
       </c>
       <c r="G47" s="0">
         <v>2</v>
@@ -21878,19 +22907,19 @@
         <v>3</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>6565</v>
+        <v>6908</v>
       </c>
       <c r="C48" s="0">
         <v>120</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>6649</v>
+        <v>6992</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>6733</v>
+        <v>7076</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>6819</v>
+        <v>7162</v>
       </c>
       <c r="G48" s="0">
         <v>3</v>
@@ -21904,19 +22933,19 @@
         <v>3</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>6566</v>
+        <v>6909</v>
       </c>
       <c r="C49" s="0">
         <v>60</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>6650</v>
+        <v>6993</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>6734</v>
+        <v>7077</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>6820</v>
+        <v>7163</v>
       </c>
       <c r="G49" s="0">
         <v>3</v>
@@ -21930,19 +22959,19 @@
         <v>2</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>6567</v>
+        <v>6910</v>
       </c>
       <c r="C50" s="0">
         <v>20</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>6651</v>
+        <v>6994</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>6735</v>
+        <v>7078</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>6821</v>
+        <v>7164</v>
       </c>
       <c r="G50" s="0">
         <v>3</v>
@@ -21956,19 +22985,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>6568</v>
+        <v>6911</v>
       </c>
       <c r="C51" s="0">
         <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>6652</v>
+        <v>6995</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>6736</v>
+        <v>7079</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>6822</v>
+        <v>7165</v>
       </c>
       <c r="G51" s="0">
         <v>4</v>
@@ -21982,19 +23011,19 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>6569</v>
+        <v>6912</v>
       </c>
       <c r="C52" s="0">
         <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>6653</v>
+        <v>6996</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>6737</v>
+        <v>7080</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>6823</v>
+        <v>7166</v>
       </c>
       <c r="G52" s="0">
         <v>4</v>
@@ -22008,19 +23037,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>6570</v>
+        <v>6913</v>
       </c>
       <c r="C53" s="0">
         <v>20</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>6653</v>
+        <v>6996</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>6738</v>
+        <v>7081</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>6824</v>
+        <v>7167</v>
       </c>
       <c r="G53" s="0">
         <v>4</v>
@@ -22034,19 +23063,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>6571</v>
+        <v>6914</v>
       </c>
       <c r="C54" s="0">
         <v>100</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>6654</v>
+        <v>6997</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>6739</v>
+        <v>7082</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>6825</v>
+        <v>7168</v>
       </c>
       <c r="G54" s="0">
         <v>0</v>
@@ -22060,19 +23089,19 @@
         <v>2</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>6571</v>
+        <v>6914</v>
       </c>
       <c r="C55" s="0">
         <v>100</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>6654</v>
+        <v>6997</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>6740</v>
+        <v>7083</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>6826</v>
+        <v>7169</v>
       </c>
       <c r="G55" s="0">
         <v>0</v>
@@ -22086,19 +23115,19 @@
         <v>3</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>6572</v>
+        <v>6915</v>
       </c>
       <c r="C56" s="0">
         <v>60</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>6655</v>
+        <v>6998</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>6741</v>
+        <v>7084</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>6827</v>
+        <v>7170</v>
       </c>
       <c r="G56" s="0">
         <v>0</v>
@@ -22112,19 +23141,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>6573</v>
+        <v>6916</v>
       </c>
       <c r="C57" s="0">
         <v>120</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>6656</v>
+        <v>6999</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>6742</v>
+        <v>7085</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>6828</v>
+        <v>7171</v>
       </c>
       <c r="G57" s="0">
         <v>1</v>
@@ -22138,19 +23167,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>6574</v>
+        <v>6917</v>
       </c>
       <c r="C58" s="0">
         <v>40</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>6657</v>
+        <v>7000</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>6743</v>
+        <v>7086</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>6829</v>
+        <v>7172</v>
       </c>
       <c r="G58" s="0">
         <v>1</v>
@@ -22164,19 +23193,19 @@
         <v>3</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>6575</v>
+        <v>6918</v>
       </c>
       <c r="C59" s="0">
         <v>20</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>6658</v>
+        <v>7001</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>6744</v>
+        <v>7087</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>6830</v>
+        <v>7173</v>
       </c>
       <c r="G59" s="0">
         <v>1</v>
@@ -22190,19 +23219,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>6576</v>
+        <v>6919</v>
       </c>
       <c r="C60" s="0">
         <v>20</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>6659</v>
+        <v>7002</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>6745</v>
+        <v>7088</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>6831</v>
+        <v>7174</v>
       </c>
       <c r="G60" s="0">
         <v>1</v>
@@ -22216,19 +23245,19 @@
         <v>3</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>6577</v>
+        <v>6920</v>
       </c>
       <c r="C61" s="0">
         <v>20</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>6660</v>
+        <v>7003</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>6746</v>
+        <v>7089</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>6832</v>
+        <v>7175</v>
       </c>
       <c r="G61" s="0">
         <v>1</v>
@@ -22242,19 +23271,19 @@
         <v>2</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>6578</v>
+        <v>6921</v>
       </c>
       <c r="C62" s="0">
         <v>40</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>6661</v>
+        <v>7004</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>6747</v>
+        <v>7090</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>6833</v>
+        <v>7176</v>
       </c>
       <c r="G62" s="0">
         <v>2</v>
@@ -22268,19 +23297,19 @@
         <v>1</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>6579</v>
+        <v>6922</v>
       </c>
       <c r="C63" s="0">
         <v>20</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>6662</v>
+        <v>7005</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>6748</v>
+        <v>7091</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>6834</v>
+        <v>7177</v>
       </c>
       <c r="G63" s="0">
         <v>2</v>
@@ -22294,19 +23323,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>6580</v>
+        <v>6923</v>
       </c>
       <c r="C64" s="0">
         <v>20</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>6663</v>
+        <v>7006</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>6749</v>
+        <v>7092</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>6835</v>
+        <v>7178</v>
       </c>
       <c r="G64" s="0">
         <v>2</v>
@@ -22320,19 +23349,19 @@
         <v>2</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>6581</v>
+        <v>6924</v>
       </c>
       <c r="C65" s="0">
         <v>100</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>6664</v>
+        <v>7007</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>6750</v>
+        <v>7093</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>6836</v>
+        <v>7179</v>
       </c>
       <c r="G65" s="0">
         <v>3</v>
@@ -22346,19 +23375,19 @@
         <v>2</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>6582</v>
+        <v>6925</v>
       </c>
       <c r="C66" s="0">
         <v>100</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>6665</v>
+        <v>7008</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>6751</v>
+        <v>7094</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>6837</v>
+        <v>7180</v>
       </c>
       <c r="G66" s="0">
         <v>3</v>
@@ -22372,19 +23401,19 @@
         <v>3</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>6583</v>
+        <v>6926</v>
       </c>
       <c r="C67" s="0">
         <v>100</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>6666</v>
+        <v>7009</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>6752</v>
+        <v>7095</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>6838</v>
+        <v>7181</v>
       </c>
       <c r="G67" s="0">
         <v>3</v>
@@ -22398,19 +23427,19 @@
         <v>3</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>6584</v>
+        <v>6927</v>
       </c>
       <c r="C68" s="0">
         <v>40</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>6667</v>
+        <v>7010</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>6753</v>
+        <v>7096</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>6839</v>
+        <v>7182</v>
       </c>
       <c r="G68" s="0">
         <v>3</v>
@@ -22424,19 +23453,19 @@
         <v>1</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>6585</v>
+        <v>6928</v>
       </c>
       <c r="C69" s="0">
         <v>20</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>6668</v>
+        <v>7011</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>6754</v>
+        <v>7097</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>6840</v>
+        <v>7183</v>
       </c>
       <c r="G69" s="0">
         <v>3</v>
@@ -22450,19 +23479,19 @@
         <v>1</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>6586</v>
+        <v>6929</v>
       </c>
       <c r="C70" s="0">
         <v>60</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>6669</v>
+        <v>7012</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>6755</v>
+        <v>7098</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>6841</v>
+        <v>7184</v>
       </c>
       <c r="G70" s="0">
         <v>4</v>
@@ -22476,19 +23505,19 @@
         <v>1</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>6587</v>
+        <v>6930</v>
       </c>
       <c r="C71" s="0">
         <v>120</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>6670</v>
+        <v>7013</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>6756</v>
+        <v>7099</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>6842</v>
+        <v>7185</v>
       </c>
       <c r="G71" s="0">
         <v>0</v>
@@ -22502,19 +23531,19 @@
         <v>2</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>6588</v>
+        <v>6931</v>
       </c>
       <c r="C72" s="0">
         <v>100</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>6671</v>
+        <v>7014</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>6757</v>
+        <v>7100</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>6843</v>
+        <v>7186</v>
       </c>
       <c r="G72" s="0">
         <v>0</v>
@@ -22528,19 +23557,19 @@
         <v>3</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>6589</v>
+        <v>6932</v>
       </c>
       <c r="C73" s="0">
         <v>60</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>6672</v>
+        <v>7015</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>6758</v>
+        <v>7101</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>6844</v>
+        <v>7187</v>
       </c>
       <c r="G73" s="0">
         <v>0</v>
@@ -22554,19 +23583,19 @@
         <v>1</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>6590</v>
+        <v>6933</v>
       </c>
       <c r="C74" s="0">
         <v>120</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>6673</v>
+        <v>7016</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>6759</v>
+        <v>7102</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>6845</v>
+        <v>7188</v>
       </c>
       <c r="G74" s="0">
         <v>1</v>
@@ -22580,19 +23609,19 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>6591</v>
+        <v>6934</v>
       </c>
       <c r="C75" s="0">
         <v>100</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>6674</v>
+        <v>7017</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>6760</v>
+        <v>7103</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>6846</v>
+        <v>7189</v>
       </c>
       <c r="G75" s="0">
         <v>1</v>
@@ -22606,19 +23635,19 @@
         <v>2</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>6592</v>
+        <v>6935</v>
       </c>
       <c r="C76" s="0">
         <v>80</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>6675</v>
+        <v>7018</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>6761</v>
+        <v>7104</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>6847</v>
+        <v>7190</v>
       </c>
       <c r="G76" s="0">
         <v>1</v>
@@ -22632,19 +23661,19 @@
         <v>2</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>6593</v>
+        <v>6936</v>
       </c>
       <c r="C77" s="0">
         <v>60</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>6676</v>
+        <v>7019</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>6762</v>
+        <v>7105</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>6848</v>
+        <v>7191</v>
       </c>
       <c r="G77" s="0">
         <v>1</v>
@@ -22658,19 +23687,19 @@
         <v>3</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>6594</v>
+        <v>6937</v>
       </c>
       <c r="C78" s="0">
         <v>60</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>6677</v>
+        <v>7020</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>6763</v>
+        <v>7106</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>6849</v>
+        <v>7192</v>
       </c>
       <c r="G78" s="0">
         <v>1</v>
@@ -22684,19 +23713,19 @@
         <v>1</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>6595</v>
+        <v>6938</v>
       </c>
       <c r="C79" s="0">
         <v>40</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>6678</v>
+        <v>7021</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>6764</v>
+        <v>7107</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>6850</v>
+        <v>7193</v>
       </c>
       <c r="G79" s="0">
         <v>1</v>
@@ -22710,19 +23739,19 @@
         <v>2</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>6596</v>
+        <v>6939</v>
       </c>
       <c r="C80" s="0">
         <v>120</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>6679</v>
+        <v>7022</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>6765</v>
+        <v>7108</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>6851</v>
+        <v>7194</v>
       </c>
       <c r="G80" s="0">
         <v>2</v>
@@ -22736,19 +23765,19 @@
         <v>1</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>6597</v>
+        <v>6940</v>
       </c>
       <c r="C81" s="0">
         <v>100</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>6680</v>
+        <v>7023</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>6766</v>
+        <v>7109</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>6852</v>
+        <v>7195</v>
       </c>
       <c r="G81" s="0">
         <v>2</v>
@@ -22762,19 +23791,19 @@
         <v>1</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>6598</v>
+        <v>6941</v>
       </c>
       <c r="C82" s="0">
         <v>60</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>6681</v>
+        <v>7024</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>6767</v>
+        <v>7110</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>6853</v>
+        <v>7196</v>
       </c>
       <c r="G82" s="0">
         <v>2</v>
@@ -22788,19 +23817,19 @@
         <v>3</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>6599</v>
+        <v>6942</v>
       </c>
       <c r="C83" s="0">
         <v>60</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>6682</v>
+        <v>7025</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>6768</v>
+        <v>7111</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>6854</v>
+        <v>7197</v>
       </c>
       <c r="G83" s="0">
         <v>2</v>
@@ -22814,19 +23843,19 @@
         <v>3</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>6600</v>
+        <v>6943</v>
       </c>
       <c r="C84" s="0">
         <v>120</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>6683</v>
+        <v>7026</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>6769</v>
+        <v>7112</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>6855</v>
+        <v>7198</v>
       </c>
       <c r="G84" s="0">
         <v>3</v>
@@ -22840,19 +23869,19 @@
         <v>2</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>6601</v>
+        <v>6944</v>
       </c>
       <c r="C85" s="0">
         <v>60</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>6684</v>
+        <v>7027</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>6770</v>
+        <v>7113</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>6856</v>
+        <v>7199</v>
       </c>
       <c r="G85" s="0">
         <v>3</v>
@@ -22866,19 +23895,19 @@
         <v>2</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>6602</v>
+        <v>6945</v>
       </c>
       <c r="C86" s="0">
         <v>20</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>6685</v>
+        <v>7028</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>6771</v>
+        <v>7114</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>6857</v>
+        <v>7200</v>
       </c>
       <c r="G86" s="0">
         <v>4</v>

</xml_diff>